<commit_message>
updated demographic data + clustering
</commit_message>
<xml_diff>
--- a/zipcodeNYC.xlsx
+++ b/zipcodeNYC.xlsx
@@ -513,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F179"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="F178" sqref="F178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4080,9 +4080,6 @@
       <c r="E178">
         <v>-73.870778999999999</v>
       </c>
-      <c r="F178" t="e">
-        <v>#N/A</v>
-      </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">

</xml_diff>